<commit_message>
modified projects, and updated project report
</commit_message>
<xml_diff>
--- a/Excel Projects/Bike Store Project.xlsx
+++ b/Excel Projects/Bike Store Project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\White\Desktop\Portfolio Projects\Excel Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA64492C-EF6F-446B-8C8C-79BA48E3F7EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB1B9AAD-6C13-4E65-BE0C-83D6C04D2D38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="working sheet" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -875,10 +875,6 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="44" applyFont="1"/>
@@ -892,6 +888,10 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -940,7 +940,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="227">
+  <dxfs count="51">
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -1071,151 +1071,7 @@
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -1225,372 +1081,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -1636,29 +1126,11 @@
         <horizontal/>
       </border>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="custom 1" pivot="0" table="0" count="10" xr9:uid="{3802D079-4339-41F2-965D-E29010E8FD8C}">
-      <tableStyleElement type="wholeTable" dxfId="220"/>
-      <tableStyleElement type="headerRow" dxfId="219"/>
+      <tableStyleElement type="wholeTable" dxfId="50"/>
+      <tableStyleElement type="headerRow" dxfId="49"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -5009,6 +4481,44 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00CC99"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-3D42-4AEC-9CCF-60F5F5C72B88}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00CC99"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-3D42-4AEC-9CCF-60F5F5C72B88}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
@@ -10684,140 +10194,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>4761</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>138111</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="29" name="TextBox 28">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F27C7D3-C94F-4198-987E-FB25E6C385B4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10906125" y="957261"/>
-          <a:ext cx="1476375" cy="323850"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>61911</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>4761</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="30" name="TextBox 29">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A347D17-65C2-4225-88C3-FB742EE26A9A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10915650" y="2538411"/>
-          <a:ext cx="1476375" cy="323850"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>228599</xdr:colOff>
       <xdr:row>6</xdr:row>
@@ -11543,73 +10919,6 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>61911</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>4761</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="48" name="TextBox 47">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A53ADBA1-D984-3F6F-B1B9-12CBE5697DA3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10896600" y="4062411"/>
-          <a:ext cx="1476375" cy="323850"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
@@ -11623,8 +10932,8 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>161926</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="50" name="Marital Status 1">
@@ -11647,7 +10956,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -11701,8 +11010,8 @@
       <xdr:row>17</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="51" name="Have Children 1">
@@ -11725,7 +11034,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -11779,8 +11088,8 @@
       <xdr:row>9</xdr:row>
       <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="52" name="Education 1">
@@ -11803,7 +11112,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -11857,8 +11166,8 @@
       <xdr:row>20</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="53" name="Home Owner 1">
@@ -11881,7 +11190,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -11935,8 +11244,8 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="54" name="Car Owner 1">
@@ -11959,7 +11268,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -12013,8 +11322,8 @@
       <xdr:row>14</xdr:row>
       <xdr:rowOff>66674</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="55" name="Region 1">
@@ -12037,7 +11346,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -12091,8 +11400,8 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="56" name="Purchased Bike 1">
@@ -12115,7 +11424,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -30273,21 +29582,64 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A94D06DA-A220-4F8C-A4FC-455F2DD3A86E}" name="PivotTable4" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="M7:O24" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{36DC745D-AAFF-48E4-A066-BEAD0D94F1A0}" name="Home Owners Per Purchase" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="I14:K18" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField showAll="0"/>
     <pivotField numFmtId="164" showAll="0"/>
     <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item m="1" x="5"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField showAll="0">
       <items count="4">
         <item x="0"/>
@@ -30297,8 +29649,15 @@
       </items>
     </pivotField>
     <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
     <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" dataField="1" showAll="0">
       <items count="3">
         <item x="0"/>
         <item x="1"/>
@@ -30306,11 +29665,34 @@
       </items>
     </pivotField>
   </pivotFields>
-  <formats count="1">
-    <format dxfId="221">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
+  <rowFields count="1">
+    <field x="8"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="15"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Purchased Bike" fld="15" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -30324,7 +29706,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DC5240D6-E456-4A95-A1D1-8E01FC64C9A9}" name="Average Income Of Bike Purchases" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DC5240D6-E456-4A95-A1D1-8E01FC64C9A9}" name="Average Income Of Bike Purchases" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A19:B22" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
@@ -30411,7 +29793,7 @@
     <dataField name="Average of Income" fld="3" subtotal="average" baseField="13" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="222">
+    <format dxfId="47">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="15" count="0"/>
@@ -30476,433 +29858,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D1C30B4B-63C1-43FD-A2AF-DA4CA2D317D6}" name="Total Count" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A1:A2" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields count="16">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of ID" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E194B4D6-FA0B-450F-8593-96BDD5C186F8}" name="Max Age" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="K1:K2" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Max of Age" fld="13" subtotal="max" baseField="0" baseItem="0" numFmtId="1"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="225">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E6796995-94DA-4195-8561-B83453A0B4B4}" name="Average Income Per Gender" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
-  <location ref="A13:B16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Average of Income" fld="3" subtotal="average" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="223">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="2" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <chartFormats count="4">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="3">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="4">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B05175A8-76EF-4FF3-8F2B-A712677D1D70}" name="Minimum Age" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="I1:I2" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Min of Age" fld="13" subtotal="min" baseField="0" baseItem="0" numFmtId="1"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="226">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3E56D688-BEF0-4C90-8290-C072BC210377}" name="Occupation" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3E56D688-BEF0-4C90-8290-C072BC210377}" name="Occupation" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="I20:J26" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
@@ -31055,318 +30011,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{36DC745D-AAFF-48E4-A066-BEAD0D94F1A0}" name="Home Owners Per Purchase" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="I14:K18" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="7">
-        <item x="0"/>
-        <item m="1" x="5"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" dataField="1" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="8"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="15"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Purchased Bike" fld="15" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1637D799-AA53-4835-AA3C-61F3FECB5F50}" name="Average Income" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="D1:D2" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Average of Income" fld="3" subtotal="average" baseField="0" baseItem="0" numFmtId="44"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="85">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B58473B4-C656-4B9E-9321-11D02DC96BC6}" name="Average Age" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="F1:F2" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Average of Age" fld="13" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="224">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DA936940-D96B-40FF-9BBE-FB4A6F21AD50}" name="Car Owners Per Purchase" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DA936940-D96B-40FF-9BBE-FB4A6F21AD50}" name="Car Owners Per Purchase" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="I7:K11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
@@ -31489,8 +30135,90 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AA7C947E-EED5-4E14-8B40-74CAE739200B}" name="Age Group DIstribution" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+<file path=xl/pivotTables/pivotTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D1C30B4B-63C1-43FD-A2AF-DA4CA2D317D6}" name="Total Count" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:A2" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="16">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of ID" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AA7C947E-EED5-4E14-8B40-74CAE739200B}" name="Age Group DIstribution" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
   <location ref="E16:F20" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
@@ -31664,8 +30392,152 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C2BF5A05-E87E-4905-A5C8-D72E43FEBF89}" name="Purchases Per Gender" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
+<file path=xl/pivotTables/pivotTable15.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A94D06DA-A220-4F8C-A4FC-455F2DD3A86E}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="M7:O24" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <formats count="1">
+    <format dxfId="48">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E194B4D6-FA0B-450F-8593-96BDD5C186F8}" name="Max Age" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="K1:K2" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Max of Age" fld="13" subtotal="max" baseField="0" baseItem="0" numFmtId="1"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="42">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C2BF5A05-E87E-4905-A5C8-D72E43FEBF89}" name="Purchases Per Gender" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
   <location ref="A6:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
@@ -31813,8 +30685,259 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{996A876F-1AED-4565-9F69-CE69A57C10BA}" name="Purchased Bikes Per Commute Distance" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1637D799-AA53-4835-AA3C-61F3FECB5F50}" name="Average Income" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="D1:D2" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of Income" fld="3" subtotal="average" baseField="0" baseItem="0" numFmtId="44"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="43">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E6796995-94DA-4195-8561-B83453A0B4B4}" name="Average Income Per Gender" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
+  <location ref="A13:B16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of Income" fld="3" subtotal="average" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="44">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="2" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <chartFormats count="4">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="4">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{996A876F-1AED-4565-9F69-CE69A57C10BA}" name="Purchased Bikes Per Commute Distance" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="E7:F13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
@@ -31951,8 +31074,101 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C8C0D780-0964-445D-8F6E-1D5C95F6A56F}" name="Marital Status" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B05175A8-76EF-4FF3-8F2B-A712677D1D70}" name="Minimum Age" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="I1:I2" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Min of Age" fld="13" subtotal="min" baseField="0" baseItem="0" numFmtId="1"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="45">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C8C0D780-0964-445D-8F6E-1D5C95F6A56F}" name="Marital Status" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="E23:G27" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
@@ -32063,6 +31279,99 @@
   <dataFields count="1">
     <dataField name="Count of Purchased Bike" fld="15" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B58473B4-C656-4B9E-9321-11D02DC96BC6}" name="Average Age" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="F1:F2" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of Age" fld="13" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="46">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -32592,7 +31901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -85717,10 +85026,10 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
+      <c r="A2" s="23">
         <v>1000</v>
       </c>
-      <c r="D2" s="23">
+      <c r="D2" s="21">
         <v>56360</v>
       </c>
       <c r="F2" s="7">
@@ -85745,7 +85054,7 @@
       <c r="A7" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="23">
         <v>489</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -85760,21 +85069,21 @@
       <c r="J7" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="M7" s="14"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="16"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="14"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="23">
         <v>511</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="23">
         <v>366</v>
       </c>
       <c r="I8" s="3" t="s">
@@ -85786,86 +85095,86 @@
       <c r="K8" t="s">
         <v>15</v>
       </c>
-      <c r="M8" s="17"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="19"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="17"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="23">
         <v>1000</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="23">
         <v>169</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="10">
+      <c r="J9" s="23">
         <v>96</v>
       </c>
-      <c r="K9" s="10">
+      <c r="K9" s="23">
         <v>151</v>
       </c>
-      <c r="M9" s="17"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="19"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="17"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="23">
         <v>162</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="10">
+      <c r="J10" s="23">
         <v>423</v>
       </c>
-      <c r="K10" s="10">
+      <c r="K10" s="23">
         <v>330</v>
       </c>
-      <c r="M10" s="17"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="19"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="17"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="23">
         <v>192</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="J11" s="10">
+      <c r="J11" s="23">
         <v>519</v>
       </c>
-      <c r="K11" s="10">
+      <c r="K11" s="23">
         <v>481</v>
       </c>
-      <c r="M11" s="17"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="19"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="17"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E12" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="23">
         <v>111</v>
       </c>
-      <c r="M12" s="17"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="19"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="17"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -85877,18 +85186,18 @@
       <c r="E13" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="23">
         <v>1000</v>
       </c>
-      <c r="M13" s="17"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="19"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="17"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="9">
         <v>54580.777096114522</v>
       </c>
       <c r="I14" s="3" t="s">
@@ -85897,15 +85206,15 @@
       <c r="J14" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="M14" s="17"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="19"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="17"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15" s="9">
         <v>58062.62230919765</v>
       </c>
       <c r="I15" s="3" t="s">
@@ -85917,15 +85226,15 @@
       <c r="K15" t="s">
         <v>15</v>
       </c>
-      <c r="M15" s="17"/>
-      <c r="N15" s="18"/>
-      <c r="O15" s="19"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="17"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="23">
         <v>56360</v>
       </c>
       <c r="E16" s="3" t="s">
@@ -85937,55 +85246,55 @@
       <c r="I16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J16" s="10">
+      <c r="J16" s="23">
         <v>161</v>
       </c>
-      <c r="K16" s="10">
+      <c r="K16" s="23">
         <v>156</v>
       </c>
-      <c r="M16" s="17"/>
-      <c r="N16" s="18"/>
-      <c r="O16" s="19"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="17"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E17" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="23">
         <v>701</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J17" s="10">
+      <c r="J17" s="23">
         <v>358</v>
       </c>
-      <c r="K17" s="10">
+      <c r="K17" s="23">
         <v>325</v>
       </c>
-      <c r="M17" s="17"/>
-      <c r="N17" s="18"/>
-      <c r="O17" s="19"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="17"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E18" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F18" s="10">
+      <c r="F18" s="23">
         <v>189</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="J18" s="10">
+      <c r="J18" s="23">
         <v>519</v>
       </c>
-      <c r="K18" s="10">
+      <c r="K18" s="23">
         <v>481</v>
       </c>
-      <c r="M18" s="17"/>
-      <c r="N18" s="18"/>
-      <c r="O18" s="19"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="17"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
@@ -85997,24 +85306,24 @@
       <c r="E19" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19" s="23">
         <v>110</v>
       </c>
-      <c r="M19" s="17"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="19"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="17"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B20" s="9">
         <v>54874.759152215796</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F20" s="23">
         <v>1000</v>
       </c>
       <c r="I20" s="3" t="s">
@@ -86023,43 +85332,43 @@
       <c r="J20" t="s">
         <v>42</v>
       </c>
-      <c r="M20" s="17"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="19"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="17"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="11">
+      <c r="B21" s="9">
         <v>57962.577962577961</v>
       </c>
       <c r="I21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J21" s="10">
+      <c r="J21" s="23">
         <v>177</v>
       </c>
-      <c r="M21" s="17"/>
-      <c r="N21" s="18"/>
-      <c r="O21" s="19"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="17"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="23">
         <v>56360</v>
       </c>
       <c r="I22" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J22" s="10">
+      <c r="J22" s="23">
         <v>173</v>
       </c>
-      <c r="M22" s="17"/>
-      <c r="N22" s="18"/>
-      <c r="O22" s="19"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="17"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E23" s="3" t="s">
@@ -86071,12 +85380,12 @@
       <c r="I23" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J23" s="10">
+      <c r="J23" s="23">
         <v>119</v>
       </c>
-      <c r="M23" s="17"/>
-      <c r="N23" s="18"/>
-      <c r="O23" s="19"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="17"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E24" s="3" t="s">
@@ -86091,27 +85400,27 @@
       <c r="I24" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J24" s="10">
+      <c r="J24" s="23">
         <v>276</v>
       </c>
-      <c r="M24" s="20"/>
-      <c r="N24" s="21"/>
-      <c r="O24" s="22"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="19"/>
+      <c r="O24" s="20"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E25" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F25" s="10">
+      <c r="F25" s="23">
         <v>307</v>
       </c>
-      <c r="G25" s="10">
+      <c r="G25" s="23">
         <v>231</v>
       </c>
       <c r="I25" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J25" s="10">
+      <c r="J25" s="23">
         <v>255</v>
       </c>
     </row>
@@ -86119,16 +85428,16 @@
       <c r="E26" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F26" s="10">
+      <c r="F26" s="23">
         <v>212</v>
       </c>
-      <c r="G26" s="10">
+      <c r="G26" s="23">
         <v>250</v>
       </c>
       <c r="I26" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="J26" s="10">
+      <c r="J26" s="23">
         <v>1000</v>
       </c>
     </row>
@@ -86136,10 +85445,10 @@
       <c r="E27" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F27" s="10">
+      <c r="F27" s="23">
         <v>519</v>
       </c>
-      <c r="G27" s="10">
+      <c r="G27" s="23">
         <v>481</v>
       </c>
     </row>
@@ -86177,26 +85486,26 @@
       <c r="A2">
         <v>1000</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="11">
         <v>56360</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="E4" s="9" t="s">
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="E4" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="I4" s="9" t="s">
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="I4" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -86280,11 +85589,11 @@
       <c r="K8" s="8"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J10" t="s">
@@ -86306,14 +85615,14 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="D12" s="9" t="s">
+      <c r="B12" s="22"/>
+      <c r="D12" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="9"/>
+      <c r="E12" s="22"/>
       <c r="J12" s="8">
         <f>J11/($J$11+$K$11)</f>
         <v>0.52415812591508049</v>
@@ -86358,17 +85667,17 @@
       <c r="E15">
         <v>162</v>
       </c>
-      <c r="I15" s="9" t="s">
+      <c r="I15" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="9"/>
+      <c r="B16" s="22"/>
       <c r="D16" s="4" t="s">
         <v>23</v>
       </c>
@@ -86434,14 +85743,14 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="9"/>
-      <c r="D20" s="9" t="s">
+      <c r="B20" s="22"/>
+      <c r="D20" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="E20" s="9"/>
+      <c r="E20" s="22"/>
       <c r="I20" t="s">
         <v>21</v>
       </c>
@@ -86499,16 +85808,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A12:B12"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="E4:G4"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -86518,19 +85827,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBEAF23C-BBA3-41BB-B8CF-488342B5B5B8}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:U1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" style="12" customWidth="1"/>
-    <col min="2" max="17" width="9.140625" style="12"/>
-    <col min="18" max="18" width="8.7109375" style="12" customWidth="1"/>
-    <col min="19" max="19" width="8.140625" style="12" customWidth="1"/>
-    <col min="20" max="20" width="7" style="12" customWidth="1"/>
-    <col min="21" max="21" width="8.140625" style="12" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="12"/>
+    <col min="1" max="1" width="8.28515625" style="10" customWidth="1"/>
+    <col min="2" max="17" width="9.140625" style="10"/>
+    <col min="18" max="18" width="8.7109375" style="10" customWidth="1"/>
+    <col min="19" max="19" width="8.140625" style="10" customWidth="1"/>
+    <col min="20" max="20" width="7" style="10" customWidth="1"/>
+    <col min="21" max="21" width="8.140625" style="10" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
modified bike store project report. Upgraded dashboard
</commit_message>
<xml_diff>
--- a/Excel Projects/Bike Store Project.xlsx
+++ b/Excel Projects/Bike Store Project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\White\Desktop\Portfolio Projects\Excel Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB1B9AAD-6C13-4E65-BE0C-83D6C04D2D38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B546E3-8ACD-4918-B79F-A0AB51612501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="working sheet" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8129" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8137" uniqueCount="63">
   <si>
     <t>ID</t>
   </si>
@@ -863,7 +863,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -892,6 +892,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -940,129 +941,9 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="51">
+  <dxfs count="9">
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -1080,13 +961,7 @@
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1129,8 +1004,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="custom 1" pivot="0" table="0" count="10" xr9:uid="{3802D079-4339-41F2-965D-E29010E8FD8C}">
-      <tableStyleElement type="wholeTable" dxfId="50"/>
-      <tableStyleElement type="headerRow" dxfId="49"/>
+      <tableStyleElement type="wholeTable" dxfId="8"/>
+      <tableStyleElement type="headerRow" dxfId="7"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -8072,6 +7947,673 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>157164</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Rectangle: Rounded Corners 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{691EA0BE-E8FB-433E-9178-D00232FE4FA7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10763250" y="504825"/>
+          <a:ext cx="1628775" cy="3843339"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 2208"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="75000"/>
+            <a:alpha val="55000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>4765</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>14290</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Graphic 12" descr="Gauge">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7917C895-6D50-4003-932B-875760B31B04}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10810875" y="766765"/>
+          <a:ext cx="581025" cy="581025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>114301</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>176216</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>76201</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>176216</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Graphic 13" descr="Table">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2B2184E-17AC-429E-AD45-0B2C90BF4676}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId4"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10820401" y="1509716"/>
+          <a:ext cx="571500" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>109540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>100015</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Graphic 14" descr="Email">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{507C07D6-00C0-4896-83E2-7CDACA9846C4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId6"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10829925" y="2205040"/>
+          <a:ext cx="561975" cy="561975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>7125</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>173815</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>138115</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Graphic 15" descr="User">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63236F16-7248-456C-BADC-F83D4129E040}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId8"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11322825" y="2840815"/>
+          <a:ext cx="535800" cy="535800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>4765</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>119065</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="TextBox 16">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E95093EC-8B55-4185-929D-066A112153EC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11382375" y="957265"/>
+          <a:ext cx="1028700" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Dashboard</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>157165</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>80965</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="TextBox 17">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87DBE57D-534E-44EB-8C13-8D18EEB20E3D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11363325" y="1681165"/>
+          <a:ext cx="1028700" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Tables</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>90490</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>14290</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="TextBox 18">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55D85847-B609-4F57-B7A9-31A79567CAC7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11372850" y="2376490"/>
+          <a:ext cx="1028700" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Feedback</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>166690</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>90490</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="TextBox 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5E51211-D0D7-4395-9C0B-CAF59E7E3F9F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11087100" y="3405190"/>
+          <a:ext cx="952500" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>linkedIn</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>138115</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>61915</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="TextBox 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB609C9F-2B41-46A1-88AB-420FE75FC333}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11077575" y="3757615"/>
+          <a:ext cx="952500" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>GitHub</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>16</xdr:row>
@@ -9370,7 +9912,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>76199</xdr:rowOff>
     </xdr:to>
@@ -9388,11 +9930,11 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10829925" y="804860"/>
-          <a:ext cx="1657350" cy="3843339"/>
+          <a:ext cx="1628775" cy="3843339"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
-            <a:gd name="adj" fmla="val 6231"/>
+            <a:gd name="adj" fmla="val 2208"/>
           </a:avLst>
         </a:prstGeom>
         <a:solidFill>
@@ -10668,15 +11210,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>352424</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
+      <xdr:colOff>476249</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -10691,8 +11233,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3857625" y="3190875"/>
-          <a:ext cx="1905000" cy="314325"/>
+          <a:off x="4562474" y="3162300"/>
+          <a:ext cx="1952625" cy="381000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -10720,7 +11262,7 @@
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
             <a:lnSpc>
               <a:spcPct val="100000"/>
             </a:lnSpc>
@@ -10746,11 +11288,30 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Total Purchase Per Gender</a:t>
+            <a:t>Customer</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1250" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> Distribution </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1250">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
-          <a:pPr marL="0" indent="0"/>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
           <a:endParaRPr lang="en-US" sz="1250">
             <a:solidFill>
               <a:schemeClr val="bg1"/>
@@ -11465,6 +12026,590 @@
     </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Graphic 10" descr="Gauge">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2A2795D-FFCD-48B2-047D-11C3BB6C2A72}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId10"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10877550" y="1066800"/>
+          <a:ext cx="581025" cy="581025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>28576</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Graphic 29" descr="Table">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A37B9B38-4275-3525-6554-7FB1EF76A544}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+          <a:extLst>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId12"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10887076" y="1809751"/>
+          <a:ext cx="571500" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="40" name="Graphic 39" descr="Email">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67BD81D7-353E-3107-1C42-9079A7AED8A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+          <a:extLst>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId14"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10896600" y="2505075"/>
+          <a:ext cx="561975" cy="561975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+            <a:prstClr val="black">
+              <a:alpha val="40000"/>
+            </a:prstClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>502425</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>92850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="49" name="Graphic 48" descr="User">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6847137F-4378-A9F5-0B16-38F9F6D5ECFE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15">
+          <a:extLst>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId16"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11389500" y="3140850"/>
+          <a:ext cx="535800" cy="535800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="57" name="TextBox 56">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02084636-6144-EB56-5DBD-D02769148875}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11449050" y="1257300"/>
+          <a:ext cx="1028700" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Dashboard</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="58" name="TextBox 57">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId18"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB84D0DF-6594-4689-98CD-ACC7563BA130}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11430000" y="1981200"/>
+          <a:ext cx="1028700" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Tables</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="59" name="TextBox 58">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId19"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D7BE91B-4D81-4197-A81C-3483FA3137CB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11439525" y="2676525"/>
+          <a:ext cx="1028700" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Feedback</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="60" name="TextBox 59">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B011A5E-D62E-40F9-B773-1B41B4FFF407}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11153775" y="3705225"/>
+          <a:ext cx="952500" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>linkedIn</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="61" name="TextBox 60">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70097DCD-F498-4BB7-94DE-8BFDCCFA68AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11144250" y="4057650"/>
+          <a:ext cx="952500" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>GitHub</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -29582,10 +30727,10 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{36DC745D-AAFF-48E4-A066-BEAD0D94F1A0}" name="Home Owners Per Purchase" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="I14:K18" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B77D5EB9-4D75-4507-B84A-10FA0ED6D794}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
+  <location ref="A30:C34" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="16">
-    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0">
       <items count="3">
         <item x="0"/>
@@ -29593,7 +30738,13 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField numFmtId="164" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0">
@@ -29614,7 +30765,7 @@
       </items>
     </pivotField>
     <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
+    <pivotField showAll="0">
       <items count="3">
         <item x="1"/>
         <item x="0"/>
@@ -29629,17 +30780,7 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0">
-      <items count="7">
-        <item x="0"/>
-        <item m="1" x="5"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
+    <pivotField showAll="0"/>
     <pivotField showAll="0">
       <items count="4">
         <item x="0"/>
@@ -29649,15 +30790,8 @@
       </items>
     </pivotField>
     <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" dataField="1" showAll="0">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
       <items count="3">
         <item x="0"/>
         <item x="1"/>
@@ -29666,7 +30800,7 @@
     </pivotField>
   </pivotFields>
   <rowFields count="1">
-    <field x="8"/>
+    <field x="2"/>
   </rowFields>
   <rowItems count="3">
     <i>
@@ -29691,7 +30825,7 @@
     </i>
   </colItems>
   <dataFields count="1">
-    <dataField name="Count of Purchased Bike" fld="15" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Count of ID" fld="0" subtotal="count" showDataAs="percentOfTotal" baseField="2" baseItem="0" numFmtId="10"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -29706,6 +30840,99 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1637D799-AA53-4835-AA3C-61F3FECB5F50}" name="Average Income" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="D1:D2" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of Income" fld="3" subtotal="average" baseField="0" baseItem="0" numFmtId="44"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="3">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DC5240D6-E456-4A95-A1D1-8E01FC64C9A9}" name="Average Income Of Bike Purchases" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A19:B22" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
@@ -29793,7 +31020,7 @@
     <dataField name="Average of Income" fld="3" subtotal="average" baseField="13" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="47">
+    <format dxfId="4">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="15" count="0"/>
@@ -29857,7 +31084,216 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A94D06DA-A220-4F8C-A4FC-455F2DD3A86E}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="M7:O24" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <formats count="1">
+    <format dxfId="5">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E6796995-94DA-4195-8561-B83453A0B4B4}" name="Average Income Per Gender" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
+  <location ref="A13:B16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of Income" fld="3" subtotal="average" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="6">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="2" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <chartFormats count="4">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="4">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable14.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3E56D688-BEF0-4C90-8290-C072BC210377}" name="Occupation" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="I20:J26" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
@@ -30011,7 +31447,362 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable15.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{996A876F-1AED-4565-9F69-CE69A57C10BA}" name="Purchased Bikes Per Commute Distance" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+  <location ref="E7:F13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item m="1" x="5"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="11"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Purchased Bike" fld="15" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="2">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable16.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{36DC745D-AAFF-48E4-A066-BEAD0D94F1A0}" name="Home Owners Per Purchase" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="I14:K18" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item m="1" x="5"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" dataField="1" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="8"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="15"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Purchased Bike" fld="15" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E194B4D6-FA0B-450F-8593-96BDD5C186F8}" name="Max Age" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="K1:K2" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Max of Age" fld="13" subtotal="max" baseField="0" baseItem="0" numFmtId="1"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="0">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DA936940-D96B-40FF-9BBE-FB4A6F21AD50}" name="Car Owners Per Purchase" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="I7:K11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="16">
@@ -30135,7 +31926,315 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B05175A8-76EF-4FF3-8F2B-A712677D1D70}" name="Minimum Age" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="I1:I2" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Min of Age" fld="13" subtotal="min" baseField="0" baseItem="0" numFmtId="1"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="1">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C2BF5A05-E87E-4905-A5C8-D72E43FEBF89}" name="Purchases Per Gender" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="11">
+  <location ref="A6:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Purchased Bike" fld="15" subtotal="count" baseField="2" baseItem="1"/>
+  </dataFields>
+  <chartFormats count="10">
+    <chartFormat chart="3" format="6" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="7">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="8">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="6" format="9" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="6" format="10">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="6" format="11">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="12" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="13">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="14">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D1C30B4B-63C1-43FD-A2AF-DA4CA2D317D6}" name="Total Count" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:A2" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="16">
@@ -30217,7 +32316,131 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C8C0D780-0964-445D-8F6E-1D5C95F6A56F}" name="Marital Status" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="E23:G27" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item m="1" x="5"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" dataField="1" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="15"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Purchased Bike" fld="15" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AA7C947E-EED5-4E14-8B40-74CAE739200B}" name="Age Group DIstribution" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
   <location ref="E16:F20" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
@@ -30392,905 +32615,6 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A94D06DA-A220-4F8C-A4FC-455F2DD3A86E}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="M7:O24" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <formats count="1">
-    <format dxfId="48">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E194B4D6-FA0B-450F-8593-96BDD5C186F8}" name="Max Age" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="K1:K2" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Max of Age" fld="13" subtotal="max" baseField="0" baseItem="0" numFmtId="1"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="42">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C2BF5A05-E87E-4905-A5C8-D72E43FEBF89}" name="Purchases Per Gender" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
-  <location ref="A6:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Purchased Bike" fld="15" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="4">
-    <chartFormat chart="3" format="6" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="7">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="8">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1637D799-AA53-4835-AA3C-61F3FECB5F50}" name="Average Income" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="D1:D2" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Average of Income" fld="3" subtotal="average" baseField="0" baseItem="0" numFmtId="44"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="43">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E6796995-94DA-4195-8561-B83453A0B4B4}" name="Average Income Per Gender" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
-  <location ref="A13:B16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Average of Income" fld="3" subtotal="average" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="44">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="2" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <chartFormats count="4">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="3">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="4">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{996A876F-1AED-4565-9F69-CE69A57C10BA}" name="Purchased Bikes Per Commute Distance" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
-  <location ref="E7:F13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="7">
-        <item x="0"/>
-        <item m="1" x="5"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="11"/>
-  </rowFields>
-  <rowItems count="6">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Purchased Bike" fld="15" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="2">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B05175A8-76EF-4FF3-8F2B-A712677D1D70}" name="Minimum Age" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="I1:I2" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Min of Age" fld="13" subtotal="min" baseField="0" baseItem="0" numFmtId="1"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="45">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C8C0D780-0964-445D-8F6E-1D5C95F6A56F}" name="Marital Status" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="E23:G27" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="7">
-        <item x="0"/>
-        <item m="1" x="5"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" dataField="1" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="15"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Purchased Bike" fld="15" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B58473B4-C656-4B9E-9321-11D02DC96BC6}" name="Average Age" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="F1:F2" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
@@ -31368,7 +32692,7 @@
     <dataField name="Average of Age" fld="13" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="46">
+    <format dxfId="2">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -31401,6 +32725,7 @@
     <pivotTable tabId="2" name="Occupation"/>
     <pivotTable tabId="2" name="Purchased Bikes Per Commute Distance"/>
     <pivotTable tabId="2" name="Total Count"/>
+    <pivotTable tabId="2" name="PivotTable3"/>
   </pivotTables>
   <data>
     <tabular pivotCacheId="75955708">
@@ -31430,6 +32755,7 @@
     <pivotTable tabId="2" name="Occupation"/>
     <pivotTable tabId="2" name="Purchased Bikes Per Commute Distance"/>
     <pivotTable tabId="2" name="Total Count"/>
+    <pivotTable tabId="2" name="PivotTable3"/>
   </pivotTables>
   <data>
     <tabular pivotCacheId="75955708">
@@ -31459,6 +32785,7 @@
     <pivotTable tabId="2" name="Occupation"/>
     <pivotTable tabId="2" name="Purchased Bikes Per Commute Distance"/>
     <pivotTable tabId="2" name="Total Count"/>
+    <pivotTable tabId="2" name="PivotTable3"/>
   </pivotTables>
   <data>
     <tabular pivotCacheId="75955708">
@@ -31491,6 +32818,7 @@
     <pivotTable tabId="2" name="Occupation"/>
     <pivotTable tabId="2" name="Purchased Bikes Per Commute Distance"/>
     <pivotTable tabId="2" name="Total Count"/>
+    <pivotTable tabId="2" name="PivotTable3"/>
   </pivotTables>
   <data>
     <tabular pivotCacheId="75955708">
@@ -31520,6 +32848,7 @@
     <pivotTable tabId="2" name="Occupation"/>
     <pivotTable tabId="2" name="Purchased Bikes Per Commute Distance"/>
     <pivotTable tabId="2" name="Total Count"/>
+    <pivotTable tabId="2" name="PivotTable3"/>
   </pivotTables>
   <data>
     <tabular pivotCacheId="75955708">
@@ -31549,6 +32878,7 @@
     <pivotTable tabId="2" name="Occupation"/>
     <pivotTable tabId="2" name="Purchased Bikes Per Commute Distance"/>
     <pivotTable tabId="2" name="Total Count"/>
+    <pivotTable tabId="2" name="PivotTable3"/>
   </pivotTables>
   <data>
     <tabular pivotCacheId="75955708">
@@ -31578,6 +32908,7 @@
     <pivotTable tabId="2" name="Minimum Age"/>
     <pivotTable tabId="2" name="Occupation"/>
     <pivotTable tabId="2" name="Purchased Bikes Per Commute Distance"/>
+    <pivotTable tabId="2" name="PivotTable3"/>
   </pivotTables>
   <data>
     <tabular pivotCacheId="75955708">
@@ -31901,7 +33232,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -84984,17 +86315,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC20F027-FE63-466C-BEB3-416CB9952B2B}">
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
@@ -85026,7 +86357,7 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="23">
+      <c r="A2">
         <v>1000</v>
       </c>
       <c r="D2" s="21">
@@ -85083,7 +86414,7 @@
       <c r="E8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8">
         <v>366</v>
       </c>
       <c r="I8" s="3" t="s">
@@ -85109,16 +86440,16 @@
       <c r="E9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="23">
+      <c r="F9">
         <v>169</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="23">
+      <c r="J9">
         <v>96</v>
       </c>
-      <c r="K9" s="23">
+      <c r="K9">
         <v>151</v>
       </c>
       <c r="M9" s="15"/>
@@ -85129,16 +86460,16 @@
       <c r="E10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="23">
+      <c r="F10">
         <v>162</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="23">
+      <c r="J10">
         <v>423</v>
       </c>
-      <c r="K10" s="23">
+      <c r="K10">
         <v>330</v>
       </c>
       <c r="M10" s="15"/>
@@ -85149,16 +86480,16 @@
       <c r="E11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="23">
+      <c r="F11">
         <v>192</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="J11" s="23">
+      <c r="J11">
         <v>519</v>
       </c>
-      <c r="K11" s="23">
+      <c r="K11">
         <v>481</v>
       </c>
       <c r="M11" s="15"/>
@@ -85169,7 +86500,7 @@
       <c r="E12" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F12" s="23">
+      <c r="F12">
         <v>111</v>
       </c>
       <c r="M12" s="15"/>
@@ -85186,7 +86517,7 @@
       <c r="E13" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="23">
+      <c r="F13">
         <v>1000</v>
       </c>
       <c r="M13" s="15"/>
@@ -85234,7 +86565,7 @@
       <c r="A16" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="23">
+      <c r="B16">
         <v>56360</v>
       </c>
       <c r="E16" s="3" t="s">
@@ -85246,10 +86577,10 @@
       <c r="I16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J16" s="23">
+      <c r="J16">
         <v>161</v>
       </c>
-      <c r="K16" s="23">
+      <c r="K16">
         <v>156</v>
       </c>
       <c r="M16" s="15"/>
@@ -85260,16 +86591,16 @@
       <c r="E17" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F17" s="23">
+      <c r="F17">
         <v>701</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J17" s="23">
+      <c r="J17">
         <v>358</v>
       </c>
-      <c r="K17" s="23">
+      <c r="K17">
         <v>325</v>
       </c>
       <c r="M17" s="15"/>
@@ -85280,16 +86611,16 @@
       <c r="E18" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F18" s="23">
+      <c r="F18">
         <v>189</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="J18" s="23">
+      <c r="J18">
         <v>519</v>
       </c>
-      <c r="K18" s="23">
+      <c r="K18">
         <v>481</v>
       </c>
       <c r="M18" s="15"/>
@@ -85306,7 +86637,7 @@
       <c r="E19" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="F19" s="23">
+      <c r="F19">
         <v>110</v>
       </c>
       <c r="M19" s="15"/>
@@ -85323,7 +86654,7 @@
       <c r="E20" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F20" s="23">
+      <c r="F20">
         <v>1000</v>
       </c>
       <c r="I20" s="3" t="s">
@@ -85346,7 +86677,7 @@
       <c r="I21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J21" s="23">
+      <c r="J21">
         <v>177</v>
       </c>
       <c r="M21" s="15"/>
@@ -85357,13 +86688,13 @@
       <c r="A22" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="23">
+      <c r="B22">
         <v>56360</v>
       </c>
       <c r="I22" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J22" s="23">
+      <c r="J22">
         <v>173</v>
       </c>
       <c r="M22" s="15"/>
@@ -85380,7 +86711,7 @@
       <c r="I23" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J23" s="23">
+      <c r="J23">
         <v>119</v>
       </c>
       <c r="M23" s="15"/>
@@ -85400,7 +86731,7 @@
       <c r="I24" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J24" s="23">
+      <c r="J24">
         <v>276</v>
       </c>
       <c r="M24" s="18"/>
@@ -85411,16 +86742,16 @@
       <c r="E25" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F25" s="23">
+      <c r="F25">
         <v>307</v>
       </c>
-      <c r="G25" s="23">
+      <c r="G25">
         <v>231</v>
       </c>
       <c r="I25" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J25" s="23">
+      <c r="J25">
         <v>255</v>
       </c>
     </row>
@@ -85428,16 +86759,16 @@
       <c r="E26" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F26" s="23">
+      <c r="F26">
         <v>212</v>
       </c>
-      <c r="G26" s="23">
+      <c r="G26">
         <v>250</v>
       </c>
       <c r="I26" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="J26" s="23">
+      <c r="J26">
         <v>1000</v>
       </c>
     </row>
@@ -85445,11 +86776,63 @@
       <c r="E27" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F27" s="23">
+      <c r="F27">
         <v>519</v>
       </c>
-      <c r="G27" s="23">
+      <c r="G27">
         <v>481</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="24">
+        <v>0.25</v>
+      </c>
+      <c r="C32" s="24">
+        <v>0.23899999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="24">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="C33" s="24">
+        <v>0.24199999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="24">
+        <v>0.51900000000000002</v>
+      </c>
+      <c r="C34" s="24">
+        <v>0.48099999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -85462,7 +86845,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B6" sqref="B6:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -85808,18 +87191,19 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="E4:G4"/>
     <mergeCell ref="I4:K4"/>
     <mergeCell ref="I9:K9"/>
     <mergeCell ref="I15:K15"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="E4:G4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -85827,9 +87211,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBEAF23C-BBA3-41BB-B8CF-488342B5B5B8}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:U1048576"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
final patch for excel file. Report is can be used
</commit_message>
<xml_diff>
--- a/Excel Projects/Bike Store Project.xlsx
+++ b/Excel Projects/Bike Store Project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\White\Desktop\Portfolio Projects\Excel Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4FAD49-6587-49EB-91F7-163BD5A77A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{993BB3D0-153D-46F5-920C-59CE01AE9017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8143" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8145" uniqueCount="63">
   <si>
     <t>ID</t>
   </si>
@@ -895,10 +895,10 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="45">
@@ -948,7 +948,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="209">
+  <dxfs count="17">
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -968,19 +968,7 @@
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -989,286 +977,13 @@
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -1314,297 +1029,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i/>
@@ -1645,12 +1069,12 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="custom 1" pivot="0" table="0" count="10" xr9:uid="{3802D079-4339-41F2-965D-E29010E8FD8C}">
-      <tableStyleElement type="wholeTable" dxfId="208"/>
-      <tableStyleElement type="headerRow" dxfId="207"/>
+      <tableStyleElement type="wholeTable" dxfId="16"/>
+      <tableStyleElement type="headerRow" dxfId="15"/>
     </tableStyle>
     <tableStyle name="custom 2" pivot="0" table="0" count="10" xr9:uid="{96E8C78D-206A-4409-86DA-01E9A4406127}">
-      <tableStyleElement type="wholeTable" dxfId="109"/>
-      <tableStyleElement type="headerRow" dxfId="108"/>
+      <tableStyleElement type="wholeTable" dxfId="14"/>
+      <tableStyleElement type="headerRow" dxfId="13"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1663,471 +1087,7 @@
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{46F421CA-312F-682f-3DD2-61675219B42D}">
-      <x14:dxfs count="32">
-        <dxf>
-          <font>
-            <color rgb="FF000000"/>
-          </font>
-          <fill>
-            <gradientFill degree="90">
-              <stop position="0">
-                <color rgb="FFF8E162"/>
-              </stop>
-              <stop position="1">
-                <color rgb="FFFCF7E0"/>
-              </stop>
-            </gradientFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color rgb="FF999999"/>
-            </left>
-            <right style="thin">
-              <color rgb="FF999999"/>
-            </right>
-            <top style="thin">
-              <color rgb="FF999999"/>
-            </top>
-            <bottom style="thin">
-              <color rgb="FF999999"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color rgb="FF000000"/>
-          </font>
-          <fill>
-            <gradientFill degree="90">
-              <stop position="0">
-                <color rgb="FFF8E162"/>
-              </stop>
-              <stop position="1">
-                <color rgb="FFFCF7E0"/>
-              </stop>
-            </gradientFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color rgb="FF999999"/>
-            </left>
-            <right style="thin">
-              <color rgb="FF999999"/>
-            </right>
-            <top style="thin">
-              <color rgb="FF999999"/>
-            </top>
-            <bottom style="thin">
-              <color rgb="FF999999"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color rgb="FF000000"/>
-          </font>
-          <fill>
-            <gradientFill degree="90">
-              <stop position="0">
-                <color rgb="FFF8E162"/>
-              </stop>
-              <stop position="1">
-                <color rgb="FFFCF7E0"/>
-              </stop>
-            </gradientFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color rgb="FF999999"/>
-            </left>
-            <right style="thin">
-              <color rgb="FF999999"/>
-            </right>
-            <top style="thin">
-              <color rgb="FF999999"/>
-            </top>
-            <bottom style="thin">
-              <color rgb="FF999999"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color rgb="FF000000"/>
-          </font>
-          <fill>
-            <gradientFill degree="90">
-              <stop position="0">
-                <color rgb="FFF8E162"/>
-              </stop>
-              <stop position="1">
-                <color rgb="FFFCF7E0"/>
-              </stop>
-            </gradientFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color rgb="FF999999"/>
-            </left>
-            <right style="thin">
-              <color rgb="FF999999"/>
-            </right>
-            <top style="thin">
-              <color rgb="FF999999"/>
-            </top>
-            <bottom style="thin">
-              <color rgb="FF999999"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color theme="8" tint="-0.249977111117893"/>
-          </font>
-          <fill>
-            <patternFill patternType="solid">
-              <fgColor theme="8" tint="0.59999389629810485"/>
-              <bgColor theme="8" tint="0.59999389629810485"/>
-            </patternFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color theme="8" tint="0.59999389629810485"/>
-            </left>
-            <right style="thin">
-              <color theme="8" tint="0.59999389629810485"/>
-            </right>
-            <top style="thin">
-              <color theme="8" tint="0.59999389629810485"/>
-            </top>
-            <bottom style="thin">
-              <color theme="8" tint="0.59999389629810485"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color theme="0"/>
-          </font>
-          <fill>
-            <patternFill patternType="solid">
-              <fgColor theme="8"/>
-              <bgColor theme="8"/>
-            </patternFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color theme="8"/>
-            </left>
-            <right style="thin">
-              <color theme="8"/>
-            </right>
-            <top style="thin">
-              <color theme="8"/>
-            </top>
-            <bottom style="thin">
-              <color theme="8"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color rgb="FF959595"/>
-          </font>
-          <fill>
-            <patternFill patternType="solid">
-              <fgColor rgb="FFDFDFDF"/>
-              <bgColor rgb="FFDFDFDF"/>
-            </patternFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color rgb="FFDFDFDF"/>
-            </left>
-            <right style="thin">
-              <color rgb="FFDFDFDF"/>
-            </right>
-            <top style="thin">
-              <color rgb="FFDFDFDF"/>
-            </top>
-            <bottom style="thin">
-              <color rgb="FFDFDFDF"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color rgb="FF000000"/>
-          </font>
-          <fill>
-            <patternFill patternType="solid">
-              <fgColor rgb="FFC0C0C0"/>
-              <bgColor rgb="FFC0C0C0"/>
-            </patternFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color rgb="FFC0C0C0"/>
-            </left>
-            <right style="thin">
-              <color rgb="FFC0C0C0"/>
-            </right>
-            <top style="thin">
-              <color rgb="FFC0C0C0"/>
-            </top>
-            <bottom style="thin">
-              <color rgb="FFC0C0C0"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color rgb="FF000000"/>
-          </font>
-          <fill>
-            <gradientFill degree="90">
-              <stop position="0">
-                <color rgb="FFF8E162"/>
-              </stop>
-              <stop position="1">
-                <color rgb="FFFCF7E0"/>
-              </stop>
-            </gradientFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color rgb="FF999999"/>
-            </left>
-            <right style="thin">
-              <color rgb="FF999999"/>
-            </right>
-            <top style="thin">
-              <color rgb="FF999999"/>
-            </top>
-            <bottom style="thin">
-              <color rgb="FF999999"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color rgb="FF000000"/>
-          </font>
-          <fill>
-            <gradientFill degree="90">
-              <stop position="0">
-                <color rgb="FFF8E162"/>
-              </stop>
-              <stop position="1">
-                <color rgb="FFFCF7E0"/>
-              </stop>
-            </gradientFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color rgb="FF999999"/>
-            </left>
-            <right style="thin">
-              <color rgb="FF999999"/>
-            </right>
-            <top style="thin">
-              <color rgb="FF999999"/>
-            </top>
-            <bottom style="thin">
-              <color rgb="FF999999"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color rgb="FF000000"/>
-          </font>
-          <fill>
-            <gradientFill degree="90">
-              <stop position="0">
-                <color rgb="FFF8E162"/>
-              </stop>
-              <stop position="1">
-                <color rgb="FFFCF7E0"/>
-              </stop>
-            </gradientFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color rgb="FF999999"/>
-            </left>
-            <right style="thin">
-              <color rgb="FF999999"/>
-            </right>
-            <top style="thin">
-              <color rgb="FF999999"/>
-            </top>
-            <bottom style="thin">
-              <color rgb="FF999999"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color rgb="FF000000"/>
-          </font>
-          <fill>
-            <gradientFill degree="90">
-              <stop position="0">
-                <color rgb="FFF8E162"/>
-              </stop>
-              <stop position="1">
-                <color rgb="FFFCF7E0"/>
-              </stop>
-            </gradientFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color rgb="FF999999"/>
-            </left>
-            <right style="thin">
-              <color rgb="FF999999"/>
-            </right>
-            <top style="thin">
-              <color rgb="FF999999"/>
-            </top>
-            <bottom style="thin">
-              <color rgb="FF999999"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color theme="8" tint="-0.249977111117893"/>
-          </font>
-          <fill>
-            <patternFill patternType="solid">
-              <fgColor theme="8" tint="0.59999389629810485"/>
-              <bgColor theme="8" tint="0.59999389629810485"/>
-            </patternFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color theme="8" tint="0.59999389629810485"/>
-            </left>
-            <right style="thin">
-              <color theme="8" tint="0.59999389629810485"/>
-            </right>
-            <top style="thin">
-              <color theme="8" tint="0.59999389629810485"/>
-            </top>
-            <bottom style="thin">
-              <color theme="8" tint="0.59999389629810485"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color theme="0"/>
-          </font>
-          <fill>
-            <patternFill patternType="solid">
-              <fgColor theme="8"/>
-              <bgColor theme="8"/>
-            </patternFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color theme="8"/>
-            </left>
-            <right style="thin">
-              <color theme="8"/>
-            </right>
-            <top style="thin">
-              <color theme="8"/>
-            </top>
-            <bottom style="thin">
-              <color theme="8"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color rgb="FF959595"/>
-          </font>
-          <fill>
-            <patternFill patternType="solid">
-              <fgColor rgb="FFDFDFDF"/>
-              <bgColor rgb="FFDFDFDF"/>
-            </patternFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color rgb="FFDFDFDF"/>
-            </left>
-            <right style="thin">
-              <color rgb="FFDFDFDF"/>
-            </right>
-            <top style="thin">
-              <color rgb="FFDFDFDF"/>
-            </top>
-            <bottom style="thin">
-              <color rgb="FFDFDFDF"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
-        <dxf>
-          <font>
-            <color rgb="FF000000"/>
-          </font>
-          <fill>
-            <patternFill patternType="solid">
-              <fgColor rgb="FFC0C0C0"/>
-              <bgColor rgb="FFC0C0C0"/>
-            </patternFill>
-          </fill>
-          <border>
-            <left style="thin">
-              <color rgb="FFC0C0C0"/>
-            </left>
-            <right style="thin">
-              <color rgb="FFC0C0C0"/>
-            </right>
-            <top style="thin">
-              <color rgb="FFC0C0C0"/>
-            </top>
-            <bottom style="thin">
-              <color rgb="FFC0C0C0"/>
-            </bottom>
-            <vertical/>
-            <horizontal/>
-          </border>
-        </dxf>
+      <x14:dxfs count="16">
         <dxf>
           <font>
             <color rgb="FF000000"/>
@@ -2527,14 +1487,14 @@
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1">
         <x14:slicerStyle name="custom 1">
           <x14:slicerStyleElements>
-            <x14:slicerStyleElement type="unselectedItemWithData" dxfId="31"/>
-            <x14:slicerStyleElement type="unselectedItemWithNoData" dxfId="30"/>
-            <x14:slicerStyleElement type="selectedItemWithData" dxfId="29"/>
-            <x14:slicerStyleElement type="selectedItemWithNoData" dxfId="28"/>
-            <x14:slicerStyleElement type="hoveredUnselectedItemWithData" dxfId="27"/>
-            <x14:slicerStyleElement type="hoveredSelectedItemWithData" dxfId="26"/>
-            <x14:slicerStyleElement type="hoveredUnselectedItemWithNoData" dxfId="25"/>
-            <x14:slicerStyleElement type="hoveredSelectedItemWithNoData" dxfId="24"/>
+            <x14:slicerStyleElement type="unselectedItemWithData" dxfId="15"/>
+            <x14:slicerStyleElement type="unselectedItemWithNoData" dxfId="14"/>
+            <x14:slicerStyleElement type="selectedItemWithData" dxfId="13"/>
+            <x14:slicerStyleElement type="selectedItemWithNoData" dxfId="12"/>
+            <x14:slicerStyleElement type="hoveredUnselectedItemWithData" dxfId="11"/>
+            <x14:slicerStyleElement type="hoveredSelectedItemWithData" dxfId="10"/>
+            <x14:slicerStyleElement type="hoveredUnselectedItemWithNoData" dxfId="9"/>
+            <x14:slicerStyleElement type="hoveredSelectedItemWithNoData" dxfId="8"/>
           </x14:slicerStyleElements>
         </x14:slicerStyle>
         <x14:slicerStyle name="custom 2">
@@ -3139,10 +2099,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>250</c:v>
+                  <c:v>489</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>212</c:v>
+                  <c:v>511</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3615,19 +2575,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>161</c:v>
+                  <c:v>366</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>81</c:v>
+                  <c:v>169</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>81</c:v>
+                  <c:v>162</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>91</c:v>
+                  <c:v>192</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>48</c:v>
+                  <c:v>111</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4076,19 +3036,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>91</c:v>
+                  <c:v>177</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>75</c:v>
+                  <c:v>173</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>77</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>109</c:v>
+                  <c:v>276</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>110</c:v>
+                  <c:v>255</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4607,13 +3567,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>329</c:v>
+                  <c:v>701</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>61</c:v>
+                  <c:v>189</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>72</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5227,10 +4187,10 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>52400</c:v>
+                  <c:v>54580.777096114522</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55047.169811320753</c:v>
+                  <c:v>58062.62230919765</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5869,10 +4829,10 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>51084.905660377357</c:v>
+                  <c:v>54874.759152215796</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55760</c:v>
+                  <c:v>57962.577962577961</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12139,7 +11099,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:pPr marL="0" indent="0" algn="ctr"/>
-            <a:t>462</a:t>
+            <a:t>1000</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="2800">
             <a:solidFill>
@@ -12288,7 +11248,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:pPr marL="0" indent="0" algn="ctr"/>
-            <a:t> $53,614.72 </a:t>
+            <a:t> $56,360.00 </a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1800">
             <a:solidFill>
@@ -12436,7 +11396,7 @@
               <a:cs typeface="Calibri"/>
             </a:rPr>
             <a:pPr algn="ctr"/>
-            <a:t>42</a:t>
+            <a:t>44</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="4000">
             <a:solidFill>
@@ -12739,7 +11699,7 @@
               <a:cs typeface="Calibri"/>
             </a:rPr>
             <a:pPr marL="0" indent="0" algn="ctr"/>
-            <a:t>78</a:t>
+            <a:t>89</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="4000" b="0" i="0" u="none" strike="noStrike">
             <a:solidFill>
@@ -32747,17 +31707,10 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1E134B8F-4926-4656-A441-675D5A9B859B}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="29">
-  <location ref="A41:C44" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3E56D688-BEF0-4C90-8290-C072BC210377}" name="Occupation" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="19">
+  <location ref="I24:J30" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item h="1" x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
+    <pivotField showAll="0"/>
     <pivotField showAll="0">
       <items count="3">
         <item x="0"/>
@@ -32765,6 +31718,7 @@
         <item t="default"/>
       </items>
     </pivotField>
+    <pivotField showAll="0"/>
     <pivotField numFmtId="164" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0">
@@ -32784,7 +31738,16 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item x="1"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField showAll="0">
       <items count="3">
         <item x="1"/>
@@ -32800,7 +31763,17 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item m="1" x="5"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField showAll="0">
       <items count="4">
         <item x="0"/>
@@ -32810,8 +31783,15 @@
       </items>
     </pivotField>
     <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0">
       <items count="3">
         <item x="0"/>
         <item x="1"/>
@@ -32820,80 +31800,36 @@
     </pivotField>
   </pivotFields>
   <rowFields count="1">
-    <field x="1"/>
+    <field x="7"/>
   </rowFields>
-  <rowItems count="2">
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="15"/>
-  </colFields>
-  <colItems count="2">
+  <rowItems count="6">
     <i>
       <x/>
     </i>
     <i>
       <x v="1"/>
     </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Count of ID" fld="0" subtotal="count" baseField="2" baseItem="0"/>
+    <dataField name="Count of Purchased Bike" fld="15" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="6">
-    <chartFormat chart="6" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="15" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="6" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="15" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="15" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="15" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="15" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="15" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="15" format="2" series="1">
+  <chartFormats count="4">
+    <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -32902,7 +31838,25 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="6" format="2" series="1">
+    <chartFormat chart="3" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="15" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="16" format="4" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -32925,18 +31879,24 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1637D799-AA53-4835-AA3C-61F3FECB5F50}" name="Average Income" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="D5:D6" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E6796995-94DA-4195-8561-B83453A0B4B4}" name="Average Income Per Gender" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
+  <location ref="A17:B20" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
     <pivotField showAll="0">
       <items count="3">
-        <item h="1" x="0"/>
+        <item x="0"/>
         <item x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField dataField="1" numFmtId="164" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0">
@@ -32991,20 +31951,79 @@
       </items>
     </pivotField>
   </pivotFields>
-  <rowItems count="1">
-    <i/>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
   </rowItems>
   <colItems count="1">
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Average of Income" fld="3" subtotal="average" baseField="0" baseItem="0" numFmtId="44"/>
+    <dataField name="Average of Income" fld="3" subtotal="average" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="204">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    <format dxfId="10">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="2" count="0"/>
+        </references>
+      </pivotArea>
     </format>
   </formats>
+  <chartFormats count="4">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="4">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -33024,7 +32043,7 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0">
       <items count="3">
-        <item h="1" x="0"/>
+        <item x="0"/>
         <item x="1"/>
         <item t="default"/>
       </items>
@@ -33156,13 +32175,637 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AA7C947E-EED5-4E14-8B40-74CAE739200B}" name="Age Group DIstribution" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12">
+  <location ref="E20:F24" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item m="1" x="5"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="14"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Purchased Bike" fld="15" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="5">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="6">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="14" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="7">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="14" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="8">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="14" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1E134B8F-4926-4656-A441-675D5A9B859B}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="29">
+  <location ref="A41:C45" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="16">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="15"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of ID" fld="0" subtotal="count" baseField="2" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="6">
+    <chartFormat chart="6" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="15" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="6" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="15" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="15" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="15" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="15" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="15" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="15" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="6" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{36DC745D-AAFF-48E4-A066-BEAD0D94F1A0}" name="Home Owners Per Purchase" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="I18:K22" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item m="1" x="5"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" dataField="1" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="8"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="15"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Purchased Bike" fld="15" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable15.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A94D06DA-A220-4F8C-A4FC-455F2DD3A86E}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="M11:O28" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <formats count="1">
+    <format dxfId="11">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable16.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E194B4D6-FA0B-450F-8593-96BDD5C186F8}" name="Max Age" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="K5:K6" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Max of Age" fld="13" subtotal="max" baseField="0" baseItem="0" numFmtId="1"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="12">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable17.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C2BF5A05-E87E-4905-A5C8-D72E43FEBF89}" name="Purchases Per Gender" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="13">
   <location ref="A10:B13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
     <pivotField showAll="0">
       <items count="3">
-        <item h="1" x="0"/>
+        <item x="0"/>
         <item x="1"/>
         <item t="default"/>
       </items>
@@ -33370,14 +33013,138 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C8C0D780-0964-445D-8F6E-1D5C95F6A56F}" name="Marital Status" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="E27:G31" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item m="1" x="5"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" dataField="1" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="15"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Purchased Bike" fld="15" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DC5240D6-E456-4A95-A1D1-8E01FC64C9A9}" name="Average Income Of Bike Purchases" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
   <location ref="A23:B26" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
     <pivotField showAll="0">
       <items count="3">
-        <item h="1" x="0"/>
+        <item x="0"/>
         <item x="1"/>
         <item t="default"/>
       </items>
@@ -33458,7 +33225,7 @@
     <dataField name="Average of Income" fld="3" subtotal="average" baseField="13" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="205">
+    <format dxfId="6">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="15" count="0"/>
@@ -33522,14 +33289,107 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B58473B4-C656-4B9E-9321-11D02DC96BC6}" name="Average Age" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="F5:F6" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of Age" fld="13" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="7">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D1C30B4B-63C1-43FD-A2AF-DA4CA2D317D6}" name="Total Count" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A5:A6" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="16">
     <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0">
       <items count="3">
-        <item h="1" x="0"/>
+        <item x="0"/>
         <item x="1"/>
         <item t="default"/>
       </items>
@@ -33604,251 +33464,14 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B77D5EB9-4D75-4507-B84A-10FA0ED6D794}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
-  <location ref="A34:C38" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B05175A8-76EF-4FF3-8F2B-A712677D1D70}" name="Minimum Age" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="I5:I6" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="16">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item h="1" x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
     <pivotField showAll="0"/>
     <pivotField showAll="0">
       <items count="3">
         <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="15"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of ID" fld="0" subtotal="count" showDataAs="percentOfTotal" baseField="2" baseItem="0" numFmtId="10"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{36DC745D-AAFF-48E4-A066-BEAD0D94F1A0}" name="Home Owners Per Purchase" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="I18:K22" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item h="1" x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="7">
-        <item x="0"/>
-        <item m="1" x="5"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" dataField="1" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="8"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="15"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Purchased Bike" fld="15" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E194B4D6-FA0B-450F-8593-96BDD5C186F8}" name="Max Age" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="K5:K6" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item h="1" x="0"/>
         <item x="1"/>
         <item t="default"/>
       </items>
@@ -33915,10 +33538,10 @@
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Max of Age" fld="13" subtotal="max" baseField="0" baseItem="0" numFmtId="1"/>
+    <dataField name="Min of Age" fld="13" subtotal="min" baseField="0" baseItem="0" numFmtId="1"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="206">
+    <format dxfId="8">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -33934,186 +33557,14 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A94D06DA-A220-4F8C-A4FC-455F2DD3A86E}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="M11:O28" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <formats count="1">
-    <format dxfId="200">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C8C0D780-0964-445D-8F6E-1D5C95F6A56F}" name="Marital Status" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="E27:G30" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item h="1" x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="7">
-        <item x="0"/>
-        <item m="1" x="5"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" dataField="1" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="2">
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="15"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Purchased Bike" fld="15" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DA936940-D96B-40FF-9BBE-FB4A6F21AD50}" name="Car Owners Per Purchase" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="I11:K15" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
     <pivotField showAll="0">
       <items count="3">
-        <item h="1" x="0"/>
+        <item x="0"/>
         <item x="1"/>
         <item t="default"/>
       </items>
@@ -34230,25 +33681,19 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E6796995-94DA-4195-8561-B83453A0B4B4}" name="Average Income Per Gender" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
-  <location ref="A17:B20" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1637D799-AA53-4835-AA3C-61F3FECB5F50}" name="Average Income" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="D5:D6" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
     <pivotField showAll="0">
-      <items count="3">
-        <item h="1" x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
       <items count="3">
         <item x="0"/>
         <item x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
+    <pivotField showAll="0"/>
     <pivotField dataField="1" numFmtId="164" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0">
@@ -34303,79 +33748,20 @@
       </items>
     </pivotField>
   </pivotFields>
-  <rowFields count="1">
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
+  <rowItems count="1">
+    <i/>
   </rowItems>
   <colItems count="1">
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Average of Income" fld="3" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="Average of Income" fld="3" subtotal="average" baseField="0" baseItem="0" numFmtId="44"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="201">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="2" count="0"/>
-        </references>
-      </pivotArea>
+    <format dxfId="9">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
-  <chartFormats count="4">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="3">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="4">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -34388,47 +33774,11 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AA7C947E-EED5-4E14-8B40-74CAE739200B}" name="Age Group DIstribution" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12">
-  <location ref="E20:F24" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B77D5EB9-4D75-4507-B84A-10FA0ED6D794}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
+  <location ref="A34:C38" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item h="1" x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0">
       <items count="3">
         <item x="0"/>
@@ -34436,318 +33786,13 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0">
-      <items count="7">
-        <item x="0"/>
-        <item m="1" x="5"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0">
       <items count="3">
         <item x="0"/>
         <item x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="14"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Purchased Bike" fld="15" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="5">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="5" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="6">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="14" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="7">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="14" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="8">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="14" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3E56D688-BEF0-4C90-8290-C072BC210377}" name="Occupation" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="19">
-  <location ref="I24:J30" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item h="1" x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="6">
-        <item x="1"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="7">
-        <item x="0"/>
-        <item m="1" x="5"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="7"/>
-  </rowFields>
-  <rowItems count="6">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Purchased Bike" fld="15" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="4">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="15" format="3" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="16" format="4" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B58473B4-C656-4B9E-9321-11D02DC96BC6}" name="Average Age" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="F5:F6" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item h="1" x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
     <pivotField numFmtId="164" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0">
@@ -34792,9 +33837,9 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField showAll="0">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
       <items count="3">
         <item x="0"/>
         <item x="1"/>
@@ -34802,113 +33847,34 @@
       </items>
     </pivotField>
   </pivotFields>
-  <rowItems count="1">
-    <i/>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
   </rowItems>
-  <colItems count="1">
-    <i/>
+  <colFields count="1">
+    <field x="15"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
   </colItems>
   <dataFields count="1">
-    <dataField name="Average of Age" fld="13" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
+    <dataField name="Count of ID" fld="0" subtotal="count" showDataAs="percentOfTotal" baseField="2" baseItem="0" numFmtId="10"/>
   </dataFields>
-  <formats count="1">
-    <format dxfId="202">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B05175A8-76EF-4FF3-8F2B-A712677D1D70}" name="Minimum Age" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="I5:I6" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item h="1" x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Min of Age" fld="13" subtotal="min" baseField="0" baseItem="0" numFmtId="1"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="203">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -34944,7 +33910,7 @@
   <data>
     <tabular pivotCacheId="75955708">
       <items count="2">
-        <i x="0"/>
+        <i x="0" s="1"/>
         <i x="1" s="1"/>
       </items>
     </tabular>
@@ -88535,7 +87501,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC20F027-FE63-466C-BEB3-416CB9952B2B}">
-  <dimension ref="A1:O44"/>
+  <dimension ref="A1:O45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N4" sqref="N4"/>
@@ -88559,10 +87525,10 @@
     <col min="15" max="15" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:15" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="1" spans="1:15" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:15" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:15" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:15" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>39</v>
@@ -88582,19 +87548,19 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="25">
-        <v>462</v>
+        <v>1000</v>
       </c>
       <c r="D6" s="21">
-        <v>53614.718614718615</v>
+        <v>56360</v>
       </c>
       <c r="F6" s="7">
-        <v>41.599567099567096</v>
+        <v>44.162999999999997</v>
       </c>
       <c r="I6" s="7">
         <v>25</v>
       </c>
       <c r="K6" s="7">
-        <v>78</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -88610,7 +87576,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="25">
-        <v>250</v>
+        <v>489</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>40</v>
@@ -88633,13 +87599,13 @@
         <v>35</v>
       </c>
       <c r="B12" s="25">
-        <v>212</v>
+        <v>511</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F12" s="25">
-        <v>161</v>
+        <v>366</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>40</v>
@@ -88659,22 +87625,22 @@
         <v>41</v>
       </c>
       <c r="B13" s="25">
-        <v>462</v>
+        <v>1000</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F13" s="25">
-        <v>81</v>
+        <v>169</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>18</v>
       </c>
       <c r="J13" s="25">
-        <v>33</v>
+        <v>96</v>
       </c>
       <c r="K13" s="25">
-        <v>67</v>
+        <v>151</v>
       </c>
       <c r="M13" s="15"/>
       <c r="N13" s="16"/>
@@ -88685,16 +87651,16 @@
         <v>22</v>
       </c>
       <c r="F14" s="25">
-        <v>81</v>
+        <v>162</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>15</v>
       </c>
       <c r="J14" s="25">
-        <v>179</v>
+        <v>423</v>
       </c>
       <c r="K14" s="25">
-        <v>183</v>
+        <v>330</v>
       </c>
       <c r="M14" s="15"/>
       <c r="N14" s="16"/>
@@ -88705,16 +87671,16 @@
         <v>23</v>
       </c>
       <c r="F15" s="25">
-        <v>91</v>
+        <v>192</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>41</v>
       </c>
       <c r="J15" s="25">
-        <v>212</v>
+        <v>519</v>
       </c>
       <c r="K15" s="25">
-        <v>250</v>
+        <v>481</v>
       </c>
       <c r="M15" s="15"/>
       <c r="N15" s="16"/>
@@ -88725,7 +87691,7 @@
         <v>50</v>
       </c>
       <c r="F16" s="25">
-        <v>48</v>
+        <v>111</v>
       </c>
       <c r="M16" s="15"/>
       <c r="N16" s="16"/>
@@ -88742,7 +87708,7 @@
         <v>41</v>
       </c>
       <c r="F17" s="25">
-        <v>462</v>
+        <v>1000</v>
       </c>
       <c r="M17" s="15"/>
       <c r="N17" s="16"/>
@@ -88753,7 +87719,7 @@
         <v>34</v>
       </c>
       <c r="B18" s="9">
-        <v>52400</v>
+        <v>54580.777096114522</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>42</v>
@@ -88770,7 +87736,7 @@
         <v>35</v>
       </c>
       <c r="B19" s="9">
-        <v>55047.169811320753</v>
+        <v>58062.62230919765</v>
       </c>
       <c r="I19" s="3" t="s">
         <v>40</v>
@@ -88790,7 +87756,7 @@
         <v>41</v>
       </c>
       <c r="B20" s="25">
-        <v>53614.718614718615</v>
+        <v>56360</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>40</v>
@@ -88802,10 +87768,10 @@
         <v>18</v>
       </c>
       <c r="J20" s="25">
-        <v>103</v>
+        <v>161</v>
       </c>
       <c r="K20" s="25">
-        <v>117</v>
+        <v>156</v>
       </c>
       <c r="M20" s="15"/>
       <c r="N20" s="16"/>
@@ -88816,16 +87782,16 @@
         <v>52</v>
       </c>
       <c r="F21" s="25">
-        <v>329</v>
+        <v>701</v>
       </c>
       <c r="I21" s="4" t="s">
         <v>15</v>
       </c>
       <c r="J21" s="25">
-        <v>109</v>
+        <v>358</v>
       </c>
       <c r="K21" s="25">
-        <v>133</v>
+        <v>325</v>
       </c>
       <c r="M21" s="15"/>
       <c r="N21" s="16"/>
@@ -88836,16 +87802,16 @@
         <v>53</v>
       </c>
       <c r="F22" s="25">
-        <v>61</v>
+        <v>189</v>
       </c>
       <c r="I22" s="4" t="s">
         <v>41</v>
       </c>
       <c r="J22" s="25">
-        <v>212</v>
+        <v>519</v>
       </c>
       <c r="K22" s="25">
-        <v>250</v>
+        <v>481</v>
       </c>
       <c r="M22" s="15"/>
       <c r="N22" s="16"/>
@@ -88862,7 +87828,7 @@
         <v>54</v>
       </c>
       <c r="F23" s="25">
-        <v>72</v>
+        <v>110</v>
       </c>
       <c r="M23" s="15"/>
       <c r="N23" s="16"/>
@@ -88873,13 +87839,13 @@
         <v>18</v>
       </c>
       <c r="B24" s="9">
-        <v>51084.905660377357</v>
+        <v>54874.759152215796</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>41</v>
       </c>
       <c r="F24" s="25">
-        <v>462</v>
+        <v>1000</v>
       </c>
       <c r="I24" s="3" t="s">
         <v>40</v>
@@ -88896,13 +87862,13 @@
         <v>15</v>
       </c>
       <c r="B25" s="9">
-        <v>55760</v>
+        <v>57962.577962577961</v>
       </c>
       <c r="I25" s="4" t="s">
         <v>20</v>
       </c>
       <c r="J25" s="25">
-        <v>91</v>
+        <v>177</v>
       </c>
       <c r="M25" s="15"/>
       <c r="N25" s="16"/>
@@ -88913,13 +87879,13 @@
         <v>41</v>
       </c>
       <c r="B26" s="25">
-        <v>53614.718614718615</v>
+        <v>56360</v>
       </c>
       <c r="I26" s="4" t="s">
         <v>28</v>
       </c>
       <c r="J26" s="25">
-        <v>75</v>
+        <v>173</v>
       </c>
       <c r="M26" s="15"/>
       <c r="N26" s="16"/>
@@ -88936,7 +87902,7 @@
         <v>25</v>
       </c>
       <c r="J27" s="25">
-        <v>77</v>
+        <v>119</v>
       </c>
       <c r="M27" s="15"/>
       <c r="N27" s="16"/>
@@ -88956,7 +87922,7 @@
         <v>21</v>
       </c>
       <c r="J28" s="25">
-        <v>109</v>
+        <v>276</v>
       </c>
       <c r="M28" s="18"/>
       <c r="N28" s="19"/>
@@ -88964,24 +87930,24 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E29" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F29" s="25">
-        <v>212</v>
+        <v>307</v>
       </c>
       <c r="G29" s="25">
-        <v>250</v>
+        <v>231</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>14</v>
       </c>
       <c r="J29" s="25">
-        <v>110</v>
+        <v>255</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E30" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F30" s="25">
         <v>212</v>
@@ -88993,7 +87959,18 @@
         <v>41</v>
       </c>
       <c r="J30" s="25">
-        <v>462</v>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E31" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F31" s="25">
+        <v>519</v>
+      </c>
+      <c r="G31" s="25">
+        <v>481</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -89020,10 +87997,10 @@
         <v>34</v>
       </c>
       <c r="B36" s="22">
-        <v>0.25757575757575757</v>
+        <v>0.25</v>
       </c>
       <c r="C36" s="22">
-        <v>0.28354978354978355</v>
+        <v>0.23899999999999999</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -89031,10 +88008,10 @@
         <v>35</v>
       </c>
       <c r="B37" s="22">
-        <v>0.20129870129870131</v>
+        <v>0.26900000000000002</v>
       </c>
       <c r="C37" s="22">
-        <v>0.25757575757575757</v>
+        <v>0.24199999999999999</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -89042,10 +88019,10 @@
         <v>41</v>
       </c>
       <c r="B38" s="22">
-        <v>0.45887445887445888</v>
+        <v>0.51900000000000002</v>
       </c>
       <c r="C38" s="22">
-        <v>0.54112554112554112</v>
+        <v>0.48099999999999998</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -89069,24 +88046,35 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B43" s="25">
-        <v>212</v>
+        <v>307</v>
       </c>
       <c r="C43" s="25">
-        <v>250</v>
+        <v>231</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B44" s="25">
         <v>212</v>
       </c>
       <c r="C44" s="25">
         <v>250</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B45" s="25">
+        <v>519</v>
+      </c>
+      <c r="C45" s="25">
+        <v>481</v>
       </c>
     </row>
   </sheetData>
@@ -89127,21 +88115,21 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="E4" s="23" t="s">
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="E4" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="I4" s="23" t="s">
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="I4" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -89225,11 +88213,11 @@
       <c r="K8" s="8"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I9" s="23" t="s">
+      <c r="I9" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J10" t="s">
@@ -89251,14 +88239,14 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="D12" s="23" t="s">
+      <c r="B12" s="24"/>
+      <c r="D12" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="23"/>
+      <c r="E12" s="24"/>
       <c r="J12" s="8">
         <f>J11/($J$11+$K$11)</f>
         <v>0.52415812591508049</v>
@@ -89303,17 +88291,17 @@
       <c r="E15">
         <v>162</v>
       </c>
-      <c r="I15" s="23" t="s">
+      <c r="I15" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="23"/>
+      <c r="B16" s="24"/>
       <c r="D16" s="4" t="s">
         <v>23</v>
       </c>
@@ -89379,14 +88367,14 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="23" t="s">
+      <c r="A20" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="23"/>
-      <c r="D20" s="23" t="s">
+      <c r="B20" s="24"/>
+      <c r="D20" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="E20" s="23"/>
+      <c r="E20" s="24"/>
       <c r="I20" t="s">
         <v>21</v>
       </c>
@@ -89444,16 +88432,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="E4:G4"/>
     <mergeCell ref="I4:K4"/>
     <mergeCell ref="I9:K9"/>
     <mergeCell ref="I15:K15"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="E4:G4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
updated bike store dashboard
</commit_message>
<xml_diff>
--- a/Excel Projects/Bike Store Project.xlsx
+++ b/Excel Projects/Bike Store Project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\White\Desktop\Portfolio Projects\Excel Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{993BB3D0-153D-46F5-920C-59CE01AE9017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57455319-73B7-4CF0-BCE4-FFB0842C2860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -869,7 +869,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -899,7 +899,6 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -948,16 +947,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="17">
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
+  <dxfs count="11">
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -972,15 +962,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -1069,12 +1050,12 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="custom 1" pivot="0" table="0" count="10" xr9:uid="{3802D079-4339-41F2-965D-E29010E8FD8C}">
-      <tableStyleElement type="wholeTable" dxfId="16"/>
-      <tableStyleElement type="headerRow" dxfId="15"/>
+      <tableStyleElement type="wholeTable" dxfId="10"/>
+      <tableStyleElement type="headerRow" dxfId="9"/>
     </tableStyle>
     <tableStyle name="custom 2" pivot="0" table="0" count="10" xr9:uid="{96E8C78D-206A-4409-86DA-01E9A4406127}">
-      <tableStyleElement type="wholeTable" dxfId="14"/>
-      <tableStyleElement type="headerRow" dxfId="13"/>
+      <tableStyleElement type="wholeTable" dxfId="8"/>
+      <tableStyleElement type="headerRow" dxfId="7"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -9594,13 +9575,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>485776</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
@@ -9672,13 +9653,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>57149</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>485775</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
@@ -9750,13 +9731,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>200025</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>80772</xdr:rowOff>
@@ -9828,13 +9809,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>90297</xdr:rowOff>
@@ -9906,13 +9887,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>80772</xdr:rowOff>
@@ -9984,13 +9965,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>80772</xdr:rowOff>
@@ -10062,13 +10043,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>228601</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>2</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>28576</xdr:rowOff>
@@ -10100,13 +10081,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>104774</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>419099</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
@@ -10138,13 +10119,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>28576</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>438150</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
@@ -10176,13 +10157,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>228601</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
@@ -10214,13 +10195,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>285749</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>161926</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>104774</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>9526</xdr:rowOff>
@@ -10252,13 +10233,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>352426</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>9526</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
@@ -10291,13 +10272,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>19051</xdr:colOff>
+      <xdr:colOff>19052</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>38099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>19051</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
@@ -10314,8 +10295,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="19051" y="38099"/>
-          <a:ext cx="12439650" cy="714376"/>
+          <a:off x="19052" y="38099"/>
+          <a:ext cx="12582524" cy="714376"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -10361,13 +10342,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>190501</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>342901</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -10445,13 +10426,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>121707</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>66674</xdr:rowOff>
@@ -10501,7 +10482,7 @@
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>314326</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -10573,13 +10554,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>342899</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>42861</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>7619</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>103821</xdr:rowOff>
@@ -10651,13 +10632,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>83343</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>42861</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>357663</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>103821</xdr:rowOff>
@@ -10729,13 +10710,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>433387</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>42861</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>98107</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>103821</xdr:rowOff>
@@ -10807,13 +10788,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>173830</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>42861</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>495299</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>103821</xdr:rowOff>
@@ -10885,14 +10866,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>523876</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>42860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:colOff>533401</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>76199</xdr:rowOff>
     </xdr:to>
@@ -10909,8 +10890,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10829925" y="804860"/>
-          <a:ext cx="1628775" cy="3843339"/>
+          <a:off x="10991851" y="804860"/>
+          <a:ext cx="1600200" cy="3843339"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -10963,13 +10944,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>438150</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -11035,13 +11016,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
@@ -11116,13 +11097,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>95249</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
@@ -11184,13 +11165,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>542926</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>571502</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
@@ -11265,13 +11246,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>119062</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>71436</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>28576</xdr:rowOff>
@@ -11333,13 +11314,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>71435</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>390525</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
@@ -11410,13 +11391,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>428624</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>128586</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>209549</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -11482,13 +11463,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>523875</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
@@ -11563,13 +11544,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>195261</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>90486</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>542925</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
@@ -11635,13 +11616,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>342901</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
@@ -11716,13 +11697,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>228599</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>33336</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>166686</xdr:rowOff>
@@ -11780,13 +11761,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>523874</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>4761</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>514350</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>138111</xdr:rowOff>
@@ -11844,13 +11825,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>314325</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>304801</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
@@ -11908,13 +11889,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>561975</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -12007,13 +11988,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>333374</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>114299</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
@@ -12090,13 +12071,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>295275</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
@@ -12189,13 +12170,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>352424</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>476249</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -12307,13 +12288,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>400050</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
@@ -12379,13 +12360,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>190499</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>123824</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
@@ -12463,18 +12444,18 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:colOff>142876</xdr:colOff>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>123826</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>276226</xdr:colOff>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>161926</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="50" name="Marital Status 1">
@@ -12497,7 +12478,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -12507,8 +12488,398 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="1676400" y="123826"/>
-              <a:ext cx="1381125" cy="609600"/>
+              <a:off x="1238251" y="3362326"/>
+              <a:ext cx="1123950" cy="609600"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>47623</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="51" name="Have Children 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DDD457E-7A13-44FE-AEAE-C552A40F8D25}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Have Children 1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="47623" y="3371850"/>
+              <a:ext cx="1228727" cy="628650"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>133348</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="52" name="Education 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AEA1E40-8609-47DB-A5E2-BFBC631937AE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Education 1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="38100" y="1466848"/>
+              <a:ext cx="2333625" cy="1066801"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="53" name="Home Owner 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7938A8E5-5E31-4429-ACF3-0984D076493D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Home Owner 1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1181100" y="3981450"/>
+              <a:ext cx="1209675" cy="657225"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>171451</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>104774</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="54" name="Car Owner 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9286312A-977E-4687-8CE5-964A2D85272C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Car Owner 1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="38100" y="3981451"/>
+              <a:ext cx="1162049" cy="657224"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>57149</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="55" name="Region 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0CD33F5-03BC-4A2D-B1E4-44F657AA0EC5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Region 1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="57149" y="2533650"/>
+              <a:ext cx="2324101" cy="838199"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -12542,23 +12913,23 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>76199</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="51" name="Have Children 1">
+            <xdr:cNvPr id="56" name="Purchased Bike 1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DDD457E-7A13-44FE-AEAE-C552A40F8D25}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FD28BD8-273B-4923-BC31-FC9BB652330E}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -12570,12 +12941,12 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
-              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Have Children 1"/>
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Purchased Bike 1"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -12585,8 +12956,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="76199" y="2743200"/>
-              <a:ext cx="1981201" cy="571500"/>
+              <a:off x="76199" y="828676"/>
+              <a:ext cx="2305051" cy="619124"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -12618,403 +12989,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>57148</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
-        <xdr:graphicFrame macro="">
-          <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="52" name="Education 1">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AEA1E40-8609-47DB-A5E2-BFBC631937AE}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvGraphicFramePr/>
-          </xdr:nvGraphicFramePr>
-          <xdr:xfrm>
-            <a:off x="0" y="0"/>
-            <a:ext cx="0" cy="0"/>
-          </xdr:xfrm>
-          <a:graphic>
-            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
-              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Education 1"/>
-            </a:graphicData>
-          </a:graphic>
-        </xdr:graphicFrame>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="0" name=""/>
-            <xdr:cNvSpPr>
-              <a:spLocks noTextEdit="1"/>
-            </xdr:cNvSpPr>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="85725" y="819148"/>
-              <a:ext cx="1952625" cy="1066801"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:prstClr val="white"/>
-            </a:solidFill>
-            <a:ln w="1">
-              <a:solidFill>
-                <a:prstClr val="green"/>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100"/>
-                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
-If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>95251</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
-        <xdr:graphicFrame macro="">
-          <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="53" name="Home Owner 1">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7938A8E5-5E31-4429-ACF3-0984D076493D}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvGraphicFramePr/>
-          </xdr:nvGraphicFramePr>
-          <xdr:xfrm>
-            <a:off x="0" y="0"/>
-            <a:ext cx="0" cy="0"/>
-          </xdr:xfrm>
-          <a:graphic>
-            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
-              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Home Owner 1"/>
-            </a:graphicData>
-          </a:graphic>
-        </xdr:graphicFrame>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="0" name=""/>
-            <xdr:cNvSpPr>
-              <a:spLocks noTextEdit="1"/>
-            </xdr:cNvSpPr>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="66675" y="3333751"/>
-              <a:ext cx="2009775" cy="600074"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:prstClr val="white"/>
-            </a:solidFill>
-            <a:ln w="1">
-              <a:solidFill>
-                <a:prstClr val="green"/>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100"/>
-                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
-If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>142876</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
-        <xdr:graphicFrame macro="">
-          <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="54" name="Car Owner 1">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9286312A-977E-4687-8CE5-964A2D85272C}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvGraphicFramePr/>
-          </xdr:nvGraphicFramePr>
-          <xdr:xfrm>
-            <a:off x="0" y="0"/>
-            <a:ext cx="0" cy="0"/>
-          </xdr:xfrm>
-          <a:graphic>
-            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
-              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Car Owner 1"/>
-            </a:graphicData>
-          </a:graphic>
-        </xdr:graphicFrame>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="0" name=""/>
-            <xdr:cNvSpPr>
-              <a:spLocks noTextEdit="1"/>
-            </xdr:cNvSpPr>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="66675" y="3952876"/>
-              <a:ext cx="1981200" cy="657224"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:prstClr val="white"/>
-            </a:solidFill>
-            <a:ln w="1">
-              <a:solidFill>
-                <a:prstClr val="green"/>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100"/>
-                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
-If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>85724</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>285749</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>66674</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
-        <xdr:graphicFrame macro="">
-          <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="55" name="Region 1">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0CD33F5-03BC-4A2D-B1E4-44F657AA0EC5}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvGraphicFramePr/>
-          </xdr:nvGraphicFramePr>
-          <xdr:xfrm>
-            <a:off x="0" y="0"/>
-            <a:ext cx="0" cy="0"/>
-          </xdr:xfrm>
-          <a:graphic>
-            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
-              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Region 1"/>
-            </a:graphicData>
-          </a:graphic>
-        </xdr:graphicFrame>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="0" name=""/>
-            <xdr:cNvSpPr>
-              <a:spLocks noTextEdit="1"/>
-            </xdr:cNvSpPr>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="85724" y="1895475"/>
-              <a:ext cx="1971675" cy="838199"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:prstClr val="white"/>
-            </a:solidFill>
-            <a:ln w="1">
-              <a:solidFill>
-                <a:prstClr val="green"/>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100"/>
-                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
-If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>57149</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>133351</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
-        <xdr:graphicFrame macro="">
-          <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="56" name="Purchased Bike 1">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FD28BD8-273B-4923-BC31-FC9BB652330E}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvGraphicFramePr/>
-          </xdr:nvGraphicFramePr>
-          <xdr:xfrm>
-            <a:off x="0" y="0"/>
-            <a:ext cx="0" cy="0"/>
-          </xdr:xfrm>
-          <a:graphic>
-            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
-              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Purchased Bike 1"/>
-            </a:graphicData>
-          </a:graphic>
-        </xdr:graphicFrame>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="0" name=""/>
-            <xdr:cNvSpPr>
-              <a:spLocks noTextEdit="1"/>
-            </xdr:cNvSpPr>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="57149" y="133351"/>
-              <a:ext cx="1619251" cy="619124"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:prstClr val="white"/>
-            </a:solidFill>
-            <a:ln w="1">
-              <a:solidFill>
-                <a:prstClr val="green"/>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100"/>
-                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
-If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
@@ -13065,13 +13046,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>18</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>1</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>95251</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>28576</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>95251</xdr:rowOff>
@@ -13122,13 +13103,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>18</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
@@ -13179,13 +13160,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>18</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>502425</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>92850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
@@ -13229,13 +13210,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
@@ -13302,13 +13283,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -13375,13 +13356,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
@@ -13448,13 +13429,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
@@ -13520,13 +13501,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>257175</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>200025</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
@@ -31707,6 +31688,443 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DA936940-D96B-40FF-9BBE-FB4A6F21AD50}" name="Car Owners Per Purchase" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="I11:K15" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item m="1" x="5"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" dataField="1" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="10"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="15"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Purchased Bike" fld="15" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D1C30B4B-63C1-43FD-A2AF-DA4CA2D317D6}" name="Total Count" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A5:A6" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="16">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of ID" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{996A876F-1AED-4565-9F69-CE69A57C10BA}" name="Purchased Bikes Per Commute Distance" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="56">
+  <location ref="E11:F17" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item m="1" x="5"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="11"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Purchased Bike" fld="15" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="2">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B05175A8-76EF-4FF3-8F2B-A712677D1D70}" name="Minimum Age" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="I5:I6" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Min of Age" fld="13" subtotal="min" baseField="0" baseItem="0" numFmtId="1"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="5">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable13.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3E56D688-BEF0-4C90-8290-C072BC210377}" name="Occupation" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="19">
   <location ref="I24:J30" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
@@ -31878,834 +32296,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E6796995-94DA-4195-8561-B83453A0B4B4}" name="Average Income Per Gender" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
-  <location ref="A17:B20" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Average of Income" fld="3" subtotal="average" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="10">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="2" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <chartFormats count="4">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="3">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="4">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{996A876F-1AED-4565-9F69-CE69A57C10BA}" name="Purchased Bikes Per Commute Distance" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="56">
-  <location ref="E11:F17" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="7">
-        <item x="0"/>
-        <item m="1" x="5"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="11"/>
-  </rowFields>
-  <rowItems count="6">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Purchased Bike" fld="15" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="2">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AA7C947E-EED5-4E14-8B40-74CAE739200B}" name="Age Group DIstribution" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12">
-  <location ref="E20:F24" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="7">
-        <item x="0"/>
-        <item m="1" x="5"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="14"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Purchased Bike" fld="15" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="5">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="5" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="6">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="14" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="7">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="14" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="8">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="14" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1E134B8F-4926-4656-A441-675D5A9B859B}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="29">
-  <location ref="A41:C45" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="16">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="15"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of ID" fld="0" subtotal="count" baseField="2" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="6">
-    <chartFormat chart="6" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="15" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="6" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="15" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="15" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="15" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="15" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="15" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="15" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="6" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{36DC745D-AAFF-48E4-A066-BEAD0D94F1A0}" name="Home Owners Per Purchase" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="I18:K22" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="7">
-        <item x="0"/>
-        <item m="1" x="5"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" dataField="1" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="8"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="15"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Purchased Bike" fld="15" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A94D06DA-A220-4F8C-A4FC-455F2DD3A86E}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="M11:O28" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <formats count="1">
-    <format dxfId="11">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable16.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E194B4D6-FA0B-450F-8593-96BDD5C186F8}" name="Max Age" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="K5:K6" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="16">
@@ -32782,7 +32373,7 @@
     <dataField name="Max of Age" fld="13" subtotal="max" baseField="0" baseItem="0" numFmtId="1"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="12">
+    <format dxfId="6">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -32798,7 +32389,131 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable15.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C8C0D780-0964-445D-8F6E-1D5C95F6A56F}" name="Marital Status" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="E27:G31" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item m="1" x="5"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" dataField="1" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="15"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Purchased Bike" fld="15" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable16.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C2BF5A05-E87E-4905-A5C8-D72E43FEBF89}" name="Purchases Per Gender" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="13">
   <location ref="A10:B13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
@@ -33013,12 +32728,12 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C8C0D780-0964-445D-8F6E-1D5C95F6A56F}" name="Marital Status" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="E27:G31" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<file path=xl/pivotTables/pivotTable17.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AA7C947E-EED5-4E14-8B40-74CAE739200B}" name="Age Group DIstribution" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12">
+  <location ref="E20:F24" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
+    <pivotField showAll="0">
       <items count="3">
         <item x="0"/>
         <item x="1"/>
@@ -33081,7 +32796,7 @@
       </items>
     </pivotField>
     <pivotField showAll="0"/>
-    <pivotField showAll="0">
+    <pivotField axis="axisRow" showAll="0">
       <items count="4">
         <item x="0"/>
         <item x="1"/>
@@ -33089,7 +32804,7 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisCol" dataField="1" showAll="0">
+    <pivotField dataField="1" showAll="0">
       <items count="3">
         <item x="0"/>
         <item x="1"/>
@@ -33098,33 +32813,84 @@
     </pivotField>
   </pivotFields>
   <rowFields count="1">
-    <field x="1"/>
+    <field x="14"/>
   </rowFields>
-  <rowItems count="3">
+  <rowItems count="4">
     <i>
       <x/>
     </i>
     <i>
       <x v="1"/>
     </i>
+    <i>
+      <x v="2"/>
+    </i>
     <i t="grand">
       <x/>
     </i>
   </rowItems>
-  <colFields count="1">
-    <field x="15"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
+  <colItems count="1">
+    <i/>
   </colItems>
   <dataFields count="1">
     <dataField name="Count of Purchased Bike" fld="15" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
+  <chartFormats count="5">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="6">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="14" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="7">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="14" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="8">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="14" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -33137,7 +32903,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DC5240D6-E456-4A95-A1D1-8E01FC64C9A9}" name="Average Income Of Bike Purchases" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
   <location ref="A23:B26" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
@@ -33225,7 +32991,7 @@
     <dataField name="Average of Income" fld="3" subtotal="average" baseField="13" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="6">
+    <format dxfId="0">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="15" count="0"/>
@@ -33289,11 +33055,18 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B58473B4-C656-4B9E-9321-11D02DC96BC6}" name="Average Age" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="F5:F6" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1E134B8F-4926-4656-A441-675D5A9B859B}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="29">
+  <location ref="A41:C45" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="16">
-    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField showAll="0">
       <items count="3">
         <item x="0"/>
@@ -33301,100 +33074,6 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Average of Age" fld="13" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="7">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D1C30B4B-63C1-43FD-A2AF-DA4CA2D317D6}" name="Total Count" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A5:A6" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields count="16">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
     <pivotField numFmtId="164" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0">
@@ -33441,199 +33120,7 @@
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of ID" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B05175A8-76EF-4FF3-8F2B-A712677D1D70}" name="Minimum Age" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="I5:I6" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Min of Age" fld="13" subtotal="min" baseField="0" baseItem="0" numFmtId="1"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="8">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DA936940-D96B-40FF-9BBE-FB4A6F21AD50}" name="Car Owners Per Purchase" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="I11:K15" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="7">
-        <item x="0"/>
-        <item m="1" x="5"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" dataField="1" showAll="0">
+    <pivotField axis="axisCol" showAll="0">
       <items count="3">
         <item x="0"/>
         <item x="1"/>
@@ -33642,7 +33129,7 @@
     </pivotField>
   </pivotFields>
   <rowFields count="1">
-    <field x="10"/>
+    <field x="1"/>
   </rowFields>
   <rowItems count="3">
     <i>
@@ -33667,8 +33154,76 @@
     </i>
   </colItems>
   <dataFields count="1">
-    <dataField name="Count of Purchased Bike" fld="15" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Count of ID" fld="0" subtotal="count" baseField="2" baseItem="0"/>
   </dataFields>
+  <chartFormats count="6">
+    <chartFormat chart="6" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="15" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="6" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="15" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="15" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="15" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="15" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="15" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="15" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="6" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -33681,7 +33236,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1637D799-AA53-4835-AA3C-61F3FECB5F50}" name="Average Income" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D5:D6" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="16">
@@ -33758,7 +33313,7 @@
     <dataField name="Average of Income" fld="3" subtotal="average" baseField="0" baseItem="0" numFmtId="44"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="9">
+    <format dxfId="1">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -33774,7 +33329,131 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{36DC745D-AAFF-48E4-A066-BEAD0D94F1A0}" name="Home Owners Per Purchase" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="I18:K22" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item m="1" x="5"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" dataField="1" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="8"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="15"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Purchased Bike" fld="15" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B77D5EB9-4D75-4507-B84A-10FA0ED6D794}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
   <location ref="A34:C38" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="16">
@@ -33875,6 +33554,308 @@
   <dataFields count="1">
     <dataField name="Count of ID" fld="0" subtotal="count" showDataAs="percentOfTotal" baseField="2" baseItem="0" numFmtId="10"/>
   </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B58473B4-C656-4B9E-9321-11D02DC96BC6}" name="Average Age" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="F5:F6" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of Age" fld="13" subtotal="average" baseField="0" baseItem="0" numFmtId="1"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="2">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E6796995-94DA-4195-8561-B83453A0B4B4}" name="Average Income Per Gender" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
+  <location ref="A17:B20" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of Income" fld="3" subtotal="average" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="3">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="2" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <chartFormats count="4">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="4">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A94D06DA-A220-4F8C-A4FC-455F2DD3A86E}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="M11:O28" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <formats count="1">
+    <format dxfId="4">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -87547,7 +87528,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="25">
+      <c r="A6">
         <v>1000</v>
       </c>
       <c r="D6" s="21">
@@ -87575,7 +87556,7 @@
       <c r="A11" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="25">
+      <c r="B11">
         <v>489</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -87598,13 +87579,13 @@
       <c r="A12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="25">
+      <c r="B12">
         <v>511</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="25">
+      <c r="F12">
         <v>366</v>
       </c>
       <c r="I12" s="3" t="s">
@@ -87624,22 +87605,22 @@
       <c r="A13" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="25">
+      <c r="B13">
         <v>1000</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="25">
+      <c r="F13">
         <v>169</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J13" s="25">
+      <c r="J13">
         <v>96</v>
       </c>
-      <c r="K13" s="25">
+      <c r="K13">
         <v>151</v>
       </c>
       <c r="M13" s="15"/>
@@ -87650,16 +87631,16 @@
       <c r="E14" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="25">
+      <c r="F14">
         <v>162</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J14" s="25">
+      <c r="J14">
         <v>423</v>
       </c>
-      <c r="K14" s="25">
+      <c r="K14">
         <v>330</v>
       </c>
       <c r="M14" s="15"/>
@@ -87670,16 +87651,16 @@
       <c r="E15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="25">
+      <c r="F15">
         <v>192</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="J15" s="25">
+      <c r="J15">
         <v>519</v>
       </c>
-      <c r="K15" s="25">
+      <c r="K15">
         <v>481</v>
       </c>
       <c r="M15" s="15"/>
@@ -87690,7 +87671,7 @@
       <c r="E16" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F16" s="25">
+      <c r="F16">
         <v>111</v>
       </c>
       <c r="M16" s="15"/>
@@ -87707,7 +87688,7 @@
       <c r="E17" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="25">
+      <c r="F17">
         <v>1000</v>
       </c>
       <c r="M17" s="15"/>
@@ -87755,7 +87736,7 @@
       <c r="A20" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="25">
+      <c r="B20">
         <v>56360</v>
       </c>
       <c r="E20" s="3" t="s">
@@ -87767,10 +87748,10 @@
       <c r="I20" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J20" s="25">
+      <c r="J20">
         <v>161</v>
       </c>
-      <c r="K20" s="25">
+      <c r="K20">
         <v>156</v>
       </c>
       <c r="M20" s="15"/>
@@ -87781,16 +87762,16 @@
       <c r="E21" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="25">
+      <c r="F21">
         <v>701</v>
       </c>
       <c r="I21" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J21" s="25">
+      <c r="J21">
         <v>358</v>
       </c>
-      <c r="K21" s="25">
+      <c r="K21">
         <v>325</v>
       </c>
       <c r="M21" s="15"/>
@@ -87801,16 +87782,16 @@
       <c r="E22" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F22" s="25">
+      <c r="F22">
         <v>189</v>
       </c>
       <c r="I22" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="J22" s="25">
+      <c r="J22">
         <v>519</v>
       </c>
-      <c r="K22" s="25">
+      <c r="K22">
         <v>481</v>
       </c>
       <c r="M22" s="15"/>
@@ -87827,7 +87808,7 @@
       <c r="E23" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="F23" s="25">
+      <c r="F23">
         <v>110</v>
       </c>
       <c r="M23" s="15"/>
@@ -87844,7 +87825,7 @@
       <c r="E24" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F24" s="25">
+      <c r="F24">
         <v>1000</v>
       </c>
       <c r="I24" s="3" t="s">
@@ -87867,7 +87848,7 @@
       <c r="I25" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J25" s="25">
+      <c r="J25">
         <v>177</v>
       </c>
       <c r="M25" s="15"/>
@@ -87878,13 +87859,13 @@
       <c r="A26" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="25">
+      <c r="B26">
         <v>56360</v>
       </c>
       <c r="I26" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J26" s="25">
+      <c r="J26">
         <v>173</v>
       </c>
       <c r="M26" s="15"/>
@@ -87901,7 +87882,7 @@
       <c r="I27" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J27" s="25">
+      <c r="J27">
         <v>119</v>
       </c>
       <c r="M27" s="15"/>
@@ -87921,7 +87902,7 @@
       <c r="I28" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J28" s="25">
+      <c r="J28">
         <v>276</v>
       </c>
       <c r="M28" s="18"/>
@@ -87932,16 +87913,16 @@
       <c r="E29" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F29" s="25">
+      <c r="F29">
         <v>307</v>
       </c>
-      <c r="G29" s="25">
+      <c r="G29">
         <v>231</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J29" s="25">
+      <c r="J29">
         <v>255</v>
       </c>
     </row>
@@ -87949,16 +87930,16 @@
       <c r="E30" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F30" s="25">
+      <c r="F30">
         <v>212</v>
       </c>
-      <c r="G30" s="25">
+      <c r="G30">
         <v>250</v>
       </c>
       <c r="I30" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="J30" s="25">
+      <c r="J30">
         <v>1000</v>
       </c>
     </row>
@@ -87966,10 +87947,10 @@
       <c r="E31" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F31" s="25">
+      <c r="F31">
         <v>519</v>
       </c>
-      <c r="G31" s="25">
+      <c r="G31">
         <v>481</v>
       </c>
     </row>
@@ -88048,10 +88029,10 @@
       <c r="A43" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B43" s="25">
+      <c r="B43">
         <v>307</v>
       </c>
-      <c r="C43" s="25">
+      <c r="C43">
         <v>231</v>
       </c>
     </row>
@@ -88059,10 +88040,10 @@
       <c r="A44" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B44" s="25">
+      <c r="B44">
         <v>212</v>
       </c>
-      <c r="C44" s="25">
+      <c r="C44">
         <v>250</v>
       </c>
     </row>
@@ -88070,10 +88051,10 @@
       <c r="A45" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B45" s="25">
+      <c r="B45">
         <v>519</v>
       </c>
-      <c r="C45" s="25">
+      <c r="C45">
         <v>481</v>
       </c>
     </row>
@@ -88432,16 +88413,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A12:B12"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="E4:G4"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -88453,18 +88434,22 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.28515625" style="10" customWidth="1"/>
-    <col min="2" max="17" width="9.140625" style="10"/>
-    <col min="18" max="18" width="8.7109375" style="10" customWidth="1"/>
-    <col min="19" max="19" width="8.140625" style="10" customWidth="1"/>
-    <col min="20" max="20" width="7" style="10" customWidth="1"/>
-    <col min="21" max="21" width="8.140625" style="10" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="10"/>
+    <col min="2" max="2" width="8.140625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" style="10" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" style="10" customWidth="1"/>
+    <col min="6" max="18" width="9.140625" style="10"/>
+    <col min="19" max="19" width="8.7109375" style="10" customWidth="1"/>
+    <col min="20" max="20" width="8.140625" style="10" customWidth="1"/>
+    <col min="21" max="21" width="7" style="10" customWidth="1"/>
+    <col min="22" max="22" width="8.140625" style="10" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>